<commit_message>
Modificacion en controladores y modelos
</commit_message>
<xml_diff>
--- a/web/archivos_generados/convenioPago43.xlsx
+++ b/web/archivos_generados/convenioPago43.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Nro</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Fecha Alta</t>
   </si>
   <si>
+    <t>Folio</t>
+  </si>
+  <si>
     <t>Familia</t>
   </si>
   <si>
@@ -41,10 +44,34 @@
     <t>Cuotas Impagas</t>
   </si>
   <si>
-    <t>sdfsdfsdf</t>
-  </si>
-  <si>
-    <t>2020-04-16</t>
+    <t>Saldo Abonado</t>
+  </si>
+  <si>
+    <t>xvxcv</t>
+  </si>
+  <si>
+    <t>01-04-2020</t>
+  </si>
+  <si>
+    <t>COSSARA MINGO</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>10-04-2020</t>
+  </si>
+  <si>
+    <t>BASCIANO</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>31-03-2020</t>
   </si>
   <si>
     <t>GENTILE</t>
@@ -53,28 +80,10 @@
     <t>NO</t>
   </si>
   <si>
-    <t>hghj</t>
-  </si>
-  <si>
-    <t>2020-04-01</t>
-  </si>
-  <si>
-    <t>DUARTE</t>
-  </si>
-  <si>
-    <t>Gentile SIn Servicios</t>
-  </si>
-  <si>
-    <t>2020-04-24</t>
-  </si>
-  <si>
-    <t>Gentile</t>
-  </si>
-  <si>
-    <t>2020-04-04</t>
-  </si>
-  <si>
-    <t>SI</t>
+    <t>dsadsa</t>
+  </si>
+  <si>
+    <t>ddd</t>
   </si>
 </sst>
 </file>
@@ -413,25 +422,27 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="16.424561" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,88 +467,112 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>4740.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>3770.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>3770.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>5000.0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>14500.0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>5000.0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -545,19 +580,89 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>8700.0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="G6">
-        <v>4</v>
+      <c r="F6">
+        <v>100000.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
       </c>
       <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>2000.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>3770.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
         <v>0</v>
       </c>
     </row>

</xml_diff>